<commit_message>
20250211 - Update data pull for simulated stream and springflow
</commit_message>
<xml_diff>
--- a/GSI_simobs_corr/flow_results.xlsx
+++ b/GSI_simobs_corr/flow_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Mac_xSSD/MWP-IHM/GSI_simobs_corr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F03E7711-84AA-4245-9987-9666658C54AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{783218F6-1017-CF48-A716-32F0FE45FEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43280" yWindow="500" windowWidth="38280" windowHeight="27160" activeTab="1" xr2:uid="{5EBD367D-6F37-E74D-8B1F-94D14E71A1B3}"/>
   </bookViews>
@@ -2878,13 +2878,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A450F092-0A0E-FC41-A0AF-3B2290DD1E00}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10:L10"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2900,7 +2900,7 @@
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3133,17 +3133,13 @@
         <v>63</v>
       </c>
       <c r="L7">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="M7">
-        <v>0.1</v>
-      </c>
-      <c r="O7" t="b">
-        <f>IF(TEXT(D7,0)="NULL",TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10</v>
       </c>
@@ -3175,17 +3171,13 @@
         <v>64</v>
       </c>
       <c r="L8">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="M8">
-        <v>0.5</v>
-      </c>
-      <c r="O8" t="b">
-        <f>IF(TEXT(D8,0)="NULL",TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3214,7 +3206,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3249,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3278,7 +3270,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3307,7 +3299,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -3336,7 +3328,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3365,7 +3357,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -3394,7 +3386,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>

</xml_diff>